<commit_message>
fix excel report and add new excel form
</commit_message>
<xml_diff>
--- a/rtw_excel_report/report_delivery_request_form/delivery_request_form.xlsx
+++ b/rtw_excel_report/report_delivery_request_form/delivery_request_form.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\odoo\rtw-custom\rtw_excel_report\report_delivery_request_form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95214DBE-9990-41D5-A745-FC05D3D0CB51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB388CD2-328E-45CA-9BE8-DD76F79E646B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F237A5B7-A27D-4811-A17B-37ED7542E636}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="17535" windowHeight="13710" xr2:uid="{F237A5B7-A27D-4811-A17B-37ED7542E636}"/>
   </bookViews>
   <sheets>
     <sheet name="配送作業依頼書" sheetId="1" r:id="rId1"/>
@@ -328,6 +328,9 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -346,9 +349,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -756,8 +756,8 @@
   </sheetPr>
   <dimension ref="A1:I1511"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18:C472"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -881,8 +881,8 @@
     </row>
     <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="28"/>
-      <c r="B9" s="37"/>
-      <c r="C9" s="37"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
       <c r="D9" s="6"/>
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
@@ -920,74 +920,74 @@
       </c>
       <c r="B12" s="24"/>
       <c r="C12" s="3"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="37"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
     </row>
     <row r="13" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="22"/>
       <c r="C13" s="16"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="37"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
     </row>
     <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="44"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37"/>
+      <c r="B14" s="37"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
     </row>
     <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="17"/>
       <c r="F15" s="18"/>
-      <c r="G15" s="43" t="s">
+      <c r="G15" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="H15" s="43"/>
+      <c r="H15" s="44"/>
       <c r="I15" s="33"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="38" t="s">
+      <c r="C16" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="38" t="s">
+      <c r="D16" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="38" t="s">
+      <c r="E16" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="38" t="s">
+      <c r="F16" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="38" t="s">
+      <c r="G16" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="H16" s="38" t="s">
+      <c r="H16" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="I16" s="38" t="s">
+      <c r="I16" s="39" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="40"/>
-      <c r="B17" s="42"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="39"/>
-      <c r="I17" s="39"/>
+      <c r="A17" s="41"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="31"/>

</xml_diff>

<commit_message>
fix excel + pdf report feedback
</commit_message>
<xml_diff>
--- a/rtw_excel_report/report_delivery_request_form/delivery_request_form.xlsx
+++ b/rtw_excel_report/report_delivery_request_form/delivery_request_form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\odoo\rtw-custom\rtw_excel_report\report_delivery_request_form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{111CF0F7-F7A1-4D30-A0D8-59B2E4322BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A60D344-CFBB-4957-BF76-0B1829740869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F237A5B7-A27D-4811-A17B-37ED7542E636}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>配送依頼書</t>
   </si>
@@ -103,6 +103,21 @@
   </si>
   <si>
     <t>配送金額合計（税抜）</t>
+  </si>
+  <si>
+    <t>配送</t>
+  </si>
+  <si>
+    <t>デポ</t>
+  </si>
+  <si>
+    <t>配送ラベル</t>
+  </si>
+  <si>
+    <t>設置先</t>
+  </si>
+  <si>
+    <t>設置先〒</t>
   </si>
 </sst>
 </file>
@@ -230,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -316,9 +331,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -349,6 +361,12 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -757,15 +775,15 @@
   <dimension ref="A1:I1511"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.625" style="30" customWidth="1"/>
-    <col min="2" max="2" width="40.625" customWidth="1"/>
+    <col min="2" max="2" width="36.625" customWidth="1"/>
     <col min="3" max="3" width="28.625" customWidth="1"/>
-    <col min="4" max="4" width="24.375" customWidth="1"/>
+    <col min="4" max="4" width="28.25" customWidth="1"/>
     <col min="5" max="5" width="11.5" customWidth="1"/>
     <col min="6" max="6" width="10.375" customWidth="1"/>
     <col min="7" max="7" width="12.875" customWidth="1"/>
@@ -781,14 +799,14 @@
       <c r="F1" s="4"/>
       <c r="G1" s="5"/>
       <c r="H1" s="6"/>
-      <c r="I1" s="34"/>
+      <c r="I1" s="33"/>
     </row>
     <row r="2" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="27"/>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="36"/>
+      <c r="C2" s="35"/>
       <c r="D2" s="7"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -864,7 +882,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="29" t="s">
         <v>8</v>
       </c>
@@ -879,10 +897,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="28"/>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
       <c r="D9" s="6"/>
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
@@ -892,7 +910,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="26"/>
       <c r="C10" s="6"/>
       <c r="E10" s="15"/>
@@ -901,95 +919,74 @@
       <c r="H10" s="10"/>
       <c r="I10" s="13"/>
     </row>
-    <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="29" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="24"/>
       <c r="C11" s="19"/>
       <c r="D11" s="32"/>
-      <c r="G11" s="6" t="s">
-        <v>13</v>
-      </c>
       <c r="H11" s="10"/>
       <c r="I11" s="5"/>
     </row>
-    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="28" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="24"/>
       <c r="C12" s="3"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-    </row>
-    <row r="13" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G12" s="45"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="45"/>
+    </row>
+    <row r="13" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="22"/>
       <c r="C13" s="16"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
-    </row>
-    <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="G13" s="45"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="45"/>
+    </row>
+    <row r="14" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
-      <c r="B14" s="37"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
-    </row>
-    <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="36"/>
+      <c r="C14" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="45"/>
+      <c r="I14" s="45"/>
+    </row>
+    <row r="15" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>26</v>
+      </c>
       <c r="B15" s="17"/>
       <c r="F15" s="18"/>
-      <c r="G15" s="44" t="s">
-        <v>24</v>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
+    </row>
+    <row r="16" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
+        <v>27</v>
       </c>
-      <c r="H15" s="44"/>
-      <c r="I15" s="33"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="39" t="s">
-        <v>15</v>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="44"/>
+    </row>
+    <row r="17" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
+        <v>29</v>
       </c>
-      <c r="B16" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="G16" s="39" t="s">
-        <v>21</v>
-      </c>
-      <c r="H16" s="39" t="s">
-        <v>22</v>
-      </c>
-      <c r="I16" s="39" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="41"/>
-      <c r="B17" s="43"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="44"/>
+    </row>
+    <row r="18" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="31"/>
       <c r="B18" s="20"/>
       <c r="C18" s="20"/>
@@ -1000,18 +997,22 @@
       <c r="H18" s="31"/>
       <c r="I18" s="31"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="31"/>
+    <row r="19" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="B19" s="20"/>
       <c r="C19" s="20"/>
       <c r="D19" s="20"/>
       <c r="E19" s="31"/>
       <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="31"/>
+      <c r="G19" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19" s="43"/>
       <c r="I19" s="31"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="31"/>
       <c r="B20" s="20"/>
       <c r="C20" s="20"/>
@@ -1023,26 +1024,44 @@
       <c r="I20" s="31"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="31"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="31"/>
+      <c r="A21" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="H21" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="I21" s="38" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="31"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
-      <c r="I22" s="31"/>
+      <c r="A22" s="40"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="39"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="31"/>
@@ -1099,28 +1118,7 @@
       <c r="H27" s="31"/>
       <c r="I27" s="31"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="31"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
-      <c r="I28" s="31"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="31"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="31"/>
-    </row>
+    <row r="28" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="31"/>
       <c r="B30" s="20"/>
@@ -17426,17 +17424,17 @@
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="B9:C9"/>
-    <mergeCell ref="G12:I14"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G15:I17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="64" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
fix feedback excel and pdf
</commit_message>
<xml_diff>
--- a/rtw_excel_report/report_delivery_request_form/delivery_request_form.xlsx
+++ b/rtw_excel_report/report_delivery_request_form/delivery_request_form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\odoo\rtw-custom\rtw_excel_report\report_delivery_request_form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{111CF0F7-F7A1-4D30-A0D8-59B2E4322BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A60D344-CFBB-4957-BF76-0B1829740869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F237A5B7-A27D-4811-A17B-37ED7542E636}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>配送依頼書</t>
   </si>
@@ -103,6 +103,21 @@
   </si>
   <si>
     <t>配送金額合計（税抜）</t>
+  </si>
+  <si>
+    <t>配送</t>
+  </si>
+  <si>
+    <t>デポ</t>
+  </si>
+  <si>
+    <t>配送ラベル</t>
+  </si>
+  <si>
+    <t>設置先</t>
+  </si>
+  <si>
+    <t>設置先〒</t>
   </si>
 </sst>
 </file>
@@ -230,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -316,9 +331,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -349,6 +361,12 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -757,15 +775,15 @@
   <dimension ref="A1:I1511"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.625" style="30" customWidth="1"/>
-    <col min="2" max="2" width="40.625" customWidth="1"/>
+    <col min="2" max="2" width="36.625" customWidth="1"/>
     <col min="3" max="3" width="28.625" customWidth="1"/>
-    <col min="4" max="4" width="24.375" customWidth="1"/>
+    <col min="4" max="4" width="28.25" customWidth="1"/>
     <col min="5" max="5" width="11.5" customWidth="1"/>
     <col min="6" max="6" width="10.375" customWidth="1"/>
     <col min="7" max="7" width="12.875" customWidth="1"/>
@@ -781,14 +799,14 @@
       <c r="F1" s="4"/>
       <c r="G1" s="5"/>
       <c r="H1" s="6"/>
-      <c r="I1" s="34"/>
+      <c r="I1" s="33"/>
     </row>
     <row r="2" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="27"/>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="36"/>
+      <c r="C2" s="35"/>
       <c r="D2" s="7"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -864,7 +882,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="29" t="s">
         <v>8</v>
       </c>
@@ -879,10 +897,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="28"/>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
       <c r="D9" s="6"/>
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
@@ -892,7 +910,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="26"/>
       <c r="C10" s="6"/>
       <c r="E10" s="15"/>
@@ -901,95 +919,74 @@
       <c r="H10" s="10"/>
       <c r="I10" s="13"/>
     </row>
-    <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="29" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="24"/>
       <c r="C11" s="19"/>
       <c r="D11" s="32"/>
-      <c r="G11" s="6" t="s">
-        <v>13</v>
-      </c>
       <c r="H11" s="10"/>
       <c r="I11" s="5"/>
     </row>
-    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="28" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="24"/>
       <c r="C12" s="3"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-    </row>
-    <row r="13" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G12" s="45"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="45"/>
+    </row>
+    <row r="13" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="22"/>
       <c r="C13" s="16"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
-    </row>
-    <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="G13" s="45"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="45"/>
+    </row>
+    <row r="14" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
-      <c r="B14" s="37"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
-    </row>
-    <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="36"/>
+      <c r="C14" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="45"/>
+      <c r="I14" s="45"/>
+    </row>
+    <row r="15" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>26</v>
+      </c>
       <c r="B15" s="17"/>
       <c r="F15" s="18"/>
-      <c r="G15" s="44" t="s">
-        <v>24</v>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
+    </row>
+    <row r="16" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
+        <v>27</v>
       </c>
-      <c r="H15" s="44"/>
-      <c r="I15" s="33"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="39" t="s">
-        <v>15</v>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="44"/>
+    </row>
+    <row r="17" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
+        <v>29</v>
       </c>
-      <c r="B16" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="G16" s="39" t="s">
-        <v>21</v>
-      </c>
-      <c r="H16" s="39" t="s">
-        <v>22</v>
-      </c>
-      <c r="I16" s="39" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="41"/>
-      <c r="B17" s="43"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="44"/>
+    </row>
+    <row r="18" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="31"/>
       <c r="B18" s="20"/>
       <c r="C18" s="20"/>
@@ -1000,18 +997,22 @@
       <c r="H18" s="31"/>
       <c r="I18" s="31"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="31"/>
+    <row r="19" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="B19" s="20"/>
       <c r="C19" s="20"/>
       <c r="D19" s="20"/>
       <c r="E19" s="31"/>
       <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="31"/>
+      <c r="G19" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19" s="43"/>
       <c r="I19" s="31"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="31"/>
       <c r="B20" s="20"/>
       <c r="C20" s="20"/>
@@ -1023,26 +1024,44 @@
       <c r="I20" s="31"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="31"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="31"/>
+      <c r="A21" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="H21" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="I21" s="38" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="31"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
-      <c r="I22" s="31"/>
+      <c r="A22" s="40"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="39"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="31"/>
@@ -1099,28 +1118,7 @@
       <c r="H27" s="31"/>
       <c r="I27" s="31"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="31"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
-      <c r="I28" s="31"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="31"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="31"/>
-    </row>
+    <row r="28" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="31"/>
       <c r="B30" s="20"/>
@@ -17426,17 +17424,17 @@
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="B9:C9"/>
-    <mergeCell ref="G12:I14"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G15:I17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="64" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
fix feedback delivery form (No.3, 7, 15, 16, 17)
</commit_message>
<xml_diff>
--- a/rtw_excel_report/report_delivery_request_form/delivery_request_form.xlsx
+++ b/rtw_excel_report/report_delivery_request_form/delivery_request_form.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\odoo\rtw-custom\rtw_excel_report\report_delivery_request_form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A60D344-CFBB-4957-BF76-0B1829740869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB64F5C-D33B-44B9-9D1A-A15D3283B8A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F237A5B7-A27D-4811-A17B-37ED7542E636}"/>
   </bookViews>
@@ -69,9 +69,6 @@
     <t>TEL／携帯</t>
   </si>
   <si>
-    <t>備考:</t>
-  </si>
-  <si>
     <t>搬入立会人</t>
   </si>
   <si>
@@ -118,6 +115,9 @@
   </si>
   <si>
     <t>設置先〒</t>
+  </si>
+  <si>
+    <t>送り状注記</t>
   </si>
 </sst>
 </file>
@@ -245,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -344,6 +344,12 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -363,10 +369,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -775,7 +778,7 @@
   <dimension ref="A1:I1511"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -899,8 +902,8 @@
     </row>
     <row r="9" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="28"/>
-      <c r="B9" s="37"/>
-      <c r="C9" s="37"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="39"/>
       <c r="D9" s="6"/>
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
@@ -923,7 +926,7 @@
       <c r="A11" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="24"/>
+      <c r="B11" s="10"/>
       <c r="C11" s="19"/>
       <c r="D11" s="32"/>
       <c r="H11" s="10"/>
@@ -935,56 +938,56 @@
       </c>
       <c r="B12" s="24"/>
       <c r="C12" s="3"/>
-      <c r="G12" s="45"/>
-      <c r="H12" s="45"/>
-      <c r="I12" s="45"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
     </row>
     <row r="13" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="22"/>
       <c r="C13" s="16"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="45"/>
-      <c r="I13" s="45"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
     </row>
     <row r="14" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="36"/>
       <c r="C14" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
-      <c r="H14" s="45"/>
-      <c r="I14" s="45"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
     </row>
     <row r="15" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" s="17"/>
       <c r="F15" s="18"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="44"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="46"/>
+      <c r="I15" s="46"/>
     </row>
     <row r="16" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
-      <c r="G16" s="44"/>
-      <c r="H16" s="44"/>
-      <c r="I16" s="44"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="46"/>
+      <c r="I16" s="46"/>
     </row>
     <row r="17" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
-      <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="44"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
     </row>
     <row r="18" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="31"/>
@@ -999,18 +1002,18 @@
     </row>
     <row r="19" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B19" s="20"/>
       <c r="C19" s="20"/>
       <c r="D19" s="20"/>
       <c r="E19" s="31"/>
       <c r="F19" s="31"/>
-      <c r="G19" s="43" t="s">
-        <v>24</v>
+      <c r="G19" s="45" t="s">
+        <v>23</v>
       </c>
-      <c r="H19" s="43"/>
-      <c r="I19" s="31"/>
+      <c r="H19" s="45"/>
+      <c r="I19" s="38"/>
     </row>
     <row r="20" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="31"/>
@@ -1021,47 +1024,47 @@
       <c r="F20" s="31"/>
       <c r="G20" s="31"/>
       <c r="H20" s="31"/>
-      <c r="I20" s="31"/>
+      <c r="I20" s="38"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="38" t="s">
+      <c r="A21" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="41" t="s">
+      <c r="C21" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="38" t="s">
+      <c r="D21" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="38" t="s">
+      <c r="E21" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="E21" s="38" t="s">
+      <c r="F21" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="F21" s="38" t="s">
+      <c r="G21" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="G21" s="38" t="s">
+      <c r="H21" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="H21" s="38" t="s">
+      <c r="I21" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="I21" s="38" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="40"/>
-      <c r="B22" s="42"/>
-      <c r="C22" s="39"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="39"/>
+      <c r="A22" s="42"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="41"/>
+      <c r="G22" s="41"/>
+      <c r="H22" s="41"/>
+      <c r="I22" s="41"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="31"/>

</xml_diff>